<commit_message>
added searchbar + aesthetics to page
</commit_message>
<xml_diff>
--- a/static/lipshades.xlsx
+++ b/static/lipshades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaseng/Documents/GitHub/capstone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaseng/Documents/GitHub/capstone/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8B464F-97E7-6C46-9412-8431E1741859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76563F55-4815-164A-A02C-340F5121BE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="500" windowWidth="33640" windowHeight="18400" xr2:uid="{894397F3-E24D-554A-81F9-D68CFB694252}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{894397F3-E24D-554A-81F9-D68CFB694252}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,190 +53,190 @@
     <t>color</t>
   </si>
   <si>
+    <t>C25A4E</t>
+  </si>
+  <si>
+    <t>9F5656</t>
+  </si>
+  <si>
+    <t>275 La Terra Attitude</t>
+  </si>
+  <si>
+    <t>product_line</t>
+  </si>
+  <si>
+    <t>intense_volume_matte</t>
+  </si>
+  <si>
+    <t>A00001</t>
+  </si>
+  <si>
+    <t>A00002</t>
+  </si>
+  <si>
+    <t>A00003</t>
+  </si>
+  <si>
+    <t>A00004</t>
+  </si>
+  <si>
+    <t>A00005</t>
+  </si>
+  <si>
+    <t>A00006</t>
+  </si>
+  <si>
+    <t>A00007</t>
+  </si>
+  <si>
+    <t>A00008</t>
+  </si>
+  <si>
+    <t>A00009</t>
+  </si>
+  <si>
+    <t>A00010</t>
+  </si>
+  <si>
+    <t>A00011</t>
+  </si>
+  <si>
+    <t>A00012</t>
+  </si>
+  <si>
+    <t>A00013</t>
+  </si>
+  <si>
+    <t>A00014</t>
+  </si>
+  <si>
+    <t>Le Nude Admirable</t>
+  </si>
+  <si>
+    <t>Le Rose Activist</t>
+  </si>
+  <si>
+    <t>Le Mauve Indomptable</t>
+  </si>
+  <si>
+    <t>Le Wood Nonchalant</t>
+  </si>
+  <si>
+    <t>Le Coral Irreverent</t>
+  </si>
+  <si>
+    <t>Le Rosy Confident</t>
+  </si>
+  <si>
+    <t>Le Plum Dominant</t>
+  </si>
+  <si>
+    <t>Le Rouge Avant-Garde</t>
+  </si>
+  <si>
+    <t>Le Rosewood Ambition</t>
+  </si>
+  <si>
+    <t>Le Carmin Courage</t>
+  </si>
+  <si>
+    <t>Le Nude Independant</t>
+  </si>
+  <si>
+    <t>Le Rouge Determination</t>
+  </si>
+  <si>
+    <t>D10E63</t>
+  </si>
+  <si>
+    <t>B84074</t>
+  </si>
+  <si>
+    <t>AB5153</t>
+  </si>
+  <si>
+    <t>FA367E</t>
+  </si>
+  <si>
+    <t>E4579A</t>
+  </si>
+  <si>
+    <t>781C44</t>
+  </si>
+  <si>
+    <t>7B0720</t>
+  </si>
+  <si>
+    <t>B12D7B</t>
+  </si>
+  <si>
+    <t>B70276</t>
+  </si>
+  <si>
+    <t>B63865</t>
+  </si>
+  <si>
+    <t>A60F28</t>
+  </si>
+  <si>
+    <t>A00015</t>
+  </si>
+  <si>
+    <t>A00016</t>
+  </si>
+  <si>
+    <t>A00017</t>
+  </si>
+  <si>
+    <t>A00018</t>
+  </si>
+  <si>
+    <t>A00019</t>
+  </si>
+  <si>
+    <t>A00020</t>
+  </si>
+  <si>
+    <t>reds_of_worth</t>
+  </si>
+  <si>
+    <t>Reds of Worth Satin Lipstick with Saturated Colour</t>
+  </si>
+  <si>
+    <t>Properous Red</t>
+  </si>
+  <si>
+    <t>Respected Red</t>
+  </si>
+  <si>
+    <t>Ambitious Red</t>
+  </si>
+  <si>
+    <t>Hopeful Red</t>
+  </si>
+  <si>
+    <t>Successful Red</t>
+  </si>
+  <si>
+    <t>A7002B</t>
+  </si>
+  <si>
+    <t>D30233</t>
+  </si>
+  <si>
+    <t>C50036</t>
+  </si>
+  <si>
+    <t>8D003A</t>
+  </si>
+  <si>
+    <t>CB0030</t>
+  </si>
+  <si>
+    <t>Lovely     Red</t>
+  </si>
+  <si>
     <t>129 Lead</t>
-  </si>
-  <si>
-    <t>C25A4E</t>
-  </si>
-  <si>
-    <t>9F5656</t>
-  </si>
-  <si>
-    <t>275 La Terra Attitude</t>
-  </si>
-  <si>
-    <t>product_line</t>
-  </si>
-  <si>
-    <t>intense_volume_matte</t>
-  </si>
-  <si>
-    <t>A00001</t>
-  </si>
-  <si>
-    <t>A00002</t>
-  </si>
-  <si>
-    <t>A00003</t>
-  </si>
-  <si>
-    <t>A00004</t>
-  </si>
-  <si>
-    <t>A00005</t>
-  </si>
-  <si>
-    <t>A00006</t>
-  </si>
-  <si>
-    <t>A00007</t>
-  </si>
-  <si>
-    <t>A00008</t>
-  </si>
-  <si>
-    <t>A00009</t>
-  </si>
-  <si>
-    <t>A00010</t>
-  </si>
-  <si>
-    <t>A00011</t>
-  </si>
-  <si>
-    <t>A00012</t>
-  </si>
-  <si>
-    <t>A00013</t>
-  </si>
-  <si>
-    <t>A00014</t>
-  </si>
-  <si>
-    <t>Le Nude Admirable</t>
-  </si>
-  <si>
-    <t>Le Rose Activist</t>
-  </si>
-  <si>
-    <t>Le Mauve Indomptable</t>
-  </si>
-  <si>
-    <t>Le Wood Nonchalant</t>
-  </si>
-  <si>
-    <t>Le Coral Irreverent</t>
-  </si>
-  <si>
-    <t>Le Rosy Confident</t>
-  </si>
-  <si>
-    <t>Le Plum Dominant</t>
-  </si>
-  <si>
-    <t>Le Rouge Avant-Garde</t>
-  </si>
-  <si>
-    <t>Le Rosewood Ambition</t>
-  </si>
-  <si>
-    <t>Le Carmin Courage</t>
-  </si>
-  <si>
-    <t>Le Nude Independant</t>
-  </si>
-  <si>
-    <t>Le Rouge Determination</t>
-  </si>
-  <si>
-    <t>D10E63</t>
-  </si>
-  <si>
-    <t>B84074</t>
-  </si>
-  <si>
-    <t>AB5153</t>
-  </si>
-  <si>
-    <t>FA367E</t>
-  </si>
-  <si>
-    <t>E4579A</t>
-  </si>
-  <si>
-    <t>781C44</t>
-  </si>
-  <si>
-    <t>7B0720</t>
-  </si>
-  <si>
-    <t>B12D7B</t>
-  </si>
-  <si>
-    <t>B70276</t>
-  </si>
-  <si>
-    <t>B63865</t>
-  </si>
-  <si>
-    <t>A60F28</t>
-  </si>
-  <si>
-    <t>A00015</t>
-  </si>
-  <si>
-    <t>A00016</t>
-  </si>
-  <si>
-    <t>A00017</t>
-  </si>
-  <si>
-    <t>A00018</t>
-  </si>
-  <si>
-    <t>A00019</t>
-  </si>
-  <si>
-    <t>A00020</t>
-  </si>
-  <si>
-    <t>reds_of_worth</t>
-  </si>
-  <si>
-    <t>Reds of Worth Satin Lipstick with Saturated Colour</t>
-  </si>
-  <si>
-    <t>Properous Red</t>
-  </si>
-  <si>
-    <t>Lovely Red</t>
-  </si>
-  <si>
-    <t>Respected Red</t>
-  </si>
-  <si>
-    <t>Ambitious Red</t>
-  </si>
-  <si>
-    <t>Hopeful Red</t>
-  </si>
-  <si>
-    <t>Successful Red</t>
-  </si>
-  <si>
-    <t>A7002B</t>
-  </si>
-  <si>
-    <t>D30233</t>
-  </si>
-  <si>
-    <t>C50036</t>
-  </si>
-  <si>
-    <t>8D003A</t>
-  </si>
-  <si>
-    <t>CB0030</t>
   </si>
 </sst>
 </file>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EEC25AA-D88A-064C-89E7-319327594E20}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -624,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -638,50 +638,50 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2">
         <v>823959</v>
@@ -689,271 +689,271 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D20" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E20" s="2">
         <v>780035</v>
@@ -961,19 +961,19 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed pathing and UI and added more products
</commit_message>
<xml_diff>
--- a/static/lipshades.xlsx
+++ b/static/lipshades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaseng/Documents/GitHub/capstone/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76563F55-4815-164A-A02C-340F5121BE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17B4813-ABB9-8644-A432-2FB22104D8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{894397F3-E24D-554A-81F9-D68CFB694252}"/>
+    <workbookView xWindow="22420" yWindow="500" windowWidth="28580" windowHeight="21100" xr2:uid="{894397F3-E24D-554A-81F9-D68CFB694252}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="309">
   <si>
     <t>product_id</t>
   </si>
@@ -233,10 +233,736 @@
     <t>CB0030</t>
   </si>
   <si>
-    <t>Lovely     Red</t>
-  </si>
-  <si>
     <t>129 Lead</t>
+  </si>
+  <si>
+    <t>A00021</t>
+  </si>
+  <si>
+    <t>A00022</t>
+  </si>
+  <si>
+    <t>A00023</t>
+  </si>
+  <si>
+    <t>A00024</t>
+  </si>
+  <si>
+    <t>A00025</t>
+  </si>
+  <si>
+    <t>A00026</t>
+  </si>
+  <si>
+    <t>A00027</t>
+  </si>
+  <si>
+    <t>A00028</t>
+  </si>
+  <si>
+    <t>A00029</t>
+  </si>
+  <si>
+    <t>A00030</t>
+  </si>
+  <si>
+    <t>A00031</t>
+  </si>
+  <si>
+    <t>A00032</t>
+  </si>
+  <si>
+    <t>A00033</t>
+  </si>
+  <si>
+    <t>A00034</t>
+  </si>
+  <si>
+    <t>A00035</t>
+  </si>
+  <si>
+    <t>A00036</t>
+  </si>
+  <si>
+    <t>A00037</t>
+  </si>
+  <si>
+    <t>sens_liq_cush</t>
+  </si>
+  <si>
+    <t>The Devil Wears Red</t>
+  </si>
+  <si>
+    <t>B32126</t>
+  </si>
+  <si>
+    <t>Urban Spice</t>
+  </si>
+  <si>
+    <t>BD4C33</t>
+  </si>
+  <si>
+    <t>BE4C4D</t>
+  </si>
+  <si>
+    <t>Red Lips Society</t>
+  </si>
+  <si>
+    <t>9D2F28</t>
+  </si>
+  <si>
+    <t>Girl Who Rules</t>
+  </si>
+  <si>
+    <t>Lovely Red</t>
+  </si>
+  <si>
+    <t>B53737</t>
+  </si>
+  <si>
+    <t>Cool Rebel</t>
+  </si>
+  <si>
+    <t>Sensational Cushion Matte Liquid Lip Tint Maybelline</t>
+  </si>
+  <si>
+    <t>Sunset Affair</t>
+  </si>
+  <si>
+    <t>C35B51</t>
+  </si>
+  <si>
+    <t>Pink Addiction</t>
+  </si>
+  <si>
+    <t>CF505C</t>
+  </si>
+  <si>
+    <t>Mauve Conture</t>
+  </si>
+  <si>
+    <t>B14454</t>
+  </si>
+  <si>
+    <t>Chestnut on Point</t>
+  </si>
+  <si>
+    <t>Love Drunk</t>
+  </si>
+  <si>
+    <t>BB4A4A</t>
+  </si>
+  <si>
+    <t>A00038</t>
+  </si>
+  <si>
+    <t>A00039</t>
+  </si>
+  <si>
+    <t>A00040</t>
+  </si>
+  <si>
+    <t>A00041</t>
+  </si>
+  <si>
+    <t>A00042</t>
+  </si>
+  <si>
+    <t>A00043</t>
+  </si>
+  <si>
+    <t>A00044</t>
+  </si>
+  <si>
+    <t>A00045</t>
+  </si>
+  <si>
+    <t>A00046</t>
+  </si>
+  <si>
+    <t>A00047</t>
+  </si>
+  <si>
+    <t>A00048</t>
+  </si>
+  <si>
+    <t>A00049</t>
+  </si>
+  <si>
+    <t>superstay_ink_crayon</t>
+  </si>
+  <si>
+    <t>Lead The Way</t>
+  </si>
+  <si>
+    <t>BF7878</t>
+  </si>
+  <si>
+    <t>Superstay Ink Crayon Maybelline Long Lasting Velvet Matte Lip Crayon Easy</t>
+  </si>
+  <si>
+    <t>Lip on Pulse</t>
+  </si>
+  <si>
+    <t>D36473</t>
+  </si>
+  <si>
+    <t>Change is Good</t>
+  </si>
+  <si>
+    <t>Hustle in Heels</t>
+  </si>
+  <si>
+    <t>BA3234</t>
+  </si>
+  <si>
+    <t>Laugh Louder</t>
+  </si>
+  <si>
+    <t>CB4C40</t>
+  </si>
+  <si>
+    <t>Make It Happen</t>
+  </si>
+  <si>
+    <t>6F1727</t>
+  </si>
+  <si>
+    <t>Enjoy The View</t>
+  </si>
+  <si>
+    <t>AC6059</t>
+  </si>
+  <si>
+    <t>Keep It Fun</t>
+  </si>
+  <si>
+    <t>D46D82</t>
+  </si>
+  <si>
+    <t>Own Your Empire</t>
+  </si>
+  <si>
+    <t>8E212D</t>
+  </si>
+  <si>
+    <t>superstay_matte_ink</t>
+  </si>
+  <si>
+    <t>690F04</t>
+  </si>
+  <si>
+    <t>Gritty</t>
+  </si>
+  <si>
+    <t>A00050</t>
+  </si>
+  <si>
+    <t>A00051</t>
+  </si>
+  <si>
+    <t>A00052</t>
+  </si>
+  <si>
+    <t>Standout</t>
+  </si>
+  <si>
+    <t>A0010B</t>
+  </si>
+  <si>
+    <t>Dauntless</t>
+  </si>
+  <si>
+    <t>660A0B</t>
+  </si>
+  <si>
+    <t>Fighter</t>
+  </si>
+  <si>
+    <t>Achiever</t>
+  </si>
+  <si>
+    <t>Extraordinary</t>
+  </si>
+  <si>
+    <t>C2818C</t>
+  </si>
+  <si>
+    <t>Dreamer</t>
+  </si>
+  <si>
+    <t>9E4449</t>
+  </si>
+  <si>
+    <t>Initiator</t>
+  </si>
+  <si>
+    <t>AF375E</t>
+  </si>
+  <si>
+    <t>Pathfinder</t>
+  </si>
+  <si>
+    <t>9F3C59</t>
+  </si>
+  <si>
+    <t>Savant</t>
+  </si>
+  <si>
+    <t>C09488</t>
+  </si>
+  <si>
+    <t>Loyalist</t>
+  </si>
+  <si>
+    <t>Seductress</t>
+  </si>
+  <si>
+    <t>AF746A</t>
+  </si>
+  <si>
+    <t>A00053</t>
+  </si>
+  <si>
+    <t>A00054</t>
+  </si>
+  <si>
+    <t>A00055</t>
+  </si>
+  <si>
+    <t>A00056</t>
+  </si>
+  <si>
+    <t>A00057</t>
+  </si>
+  <si>
+    <t>A00058</t>
+  </si>
+  <si>
+    <t>A00059</t>
+  </si>
+  <si>
+    <t>A00060</t>
+  </si>
+  <si>
+    <t>A00061</t>
+  </si>
+  <si>
+    <t>A00062</t>
+  </si>
+  <si>
+    <t>A00063</t>
+  </si>
+  <si>
+    <t>Artist</t>
+  </si>
+  <si>
+    <t>962A50</t>
+  </si>
+  <si>
+    <t>AB3427</t>
+  </si>
+  <si>
+    <t>Dancer</t>
+  </si>
+  <si>
+    <t>7A2B3C</t>
+  </si>
+  <si>
+    <t>Founder</t>
+  </si>
+  <si>
+    <t>Inspirer</t>
+  </si>
+  <si>
+    <t>DE6983</t>
+  </si>
+  <si>
+    <t>B86366</t>
+  </si>
+  <si>
+    <t>Self-Starter</t>
+  </si>
+  <si>
+    <t>9D2E23</t>
+  </si>
+  <si>
+    <t>Ground-Breaker</t>
+  </si>
+  <si>
+    <t>BC837B</t>
+  </si>
+  <si>
+    <t>Poet</t>
+  </si>
+  <si>
+    <t>A65D6C</t>
+  </si>
+  <si>
+    <t>Lover</t>
+  </si>
+  <si>
+    <t>934F56</t>
+  </si>
+  <si>
+    <t>Ringleader</t>
+  </si>
+  <si>
+    <t>A15849</t>
+  </si>
+  <si>
+    <t>Amazonian</t>
+  </si>
+  <si>
+    <t>A23646</t>
+  </si>
+  <si>
+    <t>Ruler</t>
+  </si>
+  <si>
+    <t>A00064</t>
+  </si>
+  <si>
+    <t>A00065</t>
+  </si>
+  <si>
+    <t>A00066</t>
+  </si>
+  <si>
+    <t>A00067</t>
+  </si>
+  <si>
+    <t>A00068</t>
+  </si>
+  <si>
+    <t>AD1F2F</t>
+  </si>
+  <si>
+    <t>Ambitious</t>
+  </si>
+  <si>
+    <t>A33D32</t>
+  </si>
+  <si>
+    <t>Assertive</t>
+  </si>
+  <si>
+    <t>Delicate</t>
+  </si>
+  <si>
+    <t>9E4851</t>
+  </si>
+  <si>
+    <t>Globetrotter</t>
+  </si>
+  <si>
+    <t>A44123</t>
+  </si>
+  <si>
+    <t>Seeker</t>
+  </si>
+  <si>
+    <t>AE524A</t>
+  </si>
+  <si>
+    <t>Versatile</t>
+  </si>
+  <si>
+    <t>Pioneer</t>
+  </si>
+  <si>
+    <t>9E2530</t>
+  </si>
+  <si>
+    <t>A00069</t>
+  </si>
+  <si>
+    <t>A00070</t>
+  </si>
+  <si>
+    <t>Two Eighty Five</t>
+  </si>
+  <si>
+    <t>A00071</t>
+  </si>
+  <si>
+    <t>A00072</t>
+  </si>
+  <si>
+    <t>A00073</t>
+  </si>
+  <si>
+    <t>A00074</t>
+  </si>
+  <si>
+    <t>A00075</t>
+  </si>
+  <si>
+    <t>A00076</t>
+  </si>
+  <si>
+    <t>A00077</t>
+  </si>
+  <si>
+    <t>A00078</t>
+  </si>
+  <si>
+    <t>A00079</t>
+  </si>
+  <si>
+    <t>A00080</t>
+  </si>
+  <si>
+    <t>A00081</t>
+  </si>
+  <si>
+    <t>superstay_vinyl_ink</t>
+  </si>
+  <si>
+    <t>Red Hot</t>
+  </si>
+  <si>
+    <t>E21011</t>
+  </si>
+  <si>
+    <t>970F22</t>
+  </si>
+  <si>
+    <t>Lippy</t>
+  </si>
+  <si>
+    <t>C25253</t>
+  </si>
+  <si>
+    <t>Peachy</t>
+  </si>
+  <si>
+    <t>Superstay Matte Ink Intense Maybelline</t>
+  </si>
+  <si>
+    <t>Superstay Vinyl Ink Longwear Liquid Lipcolor Maybelline</t>
+  </si>
+  <si>
+    <t>Coy</t>
+  </si>
+  <si>
+    <t>C14862</t>
+  </si>
+  <si>
+    <t>88092D</t>
+  </si>
+  <si>
+    <t>Unrivaled</t>
+  </si>
+  <si>
+    <t>8D464C</t>
+  </si>
+  <si>
+    <t>Witty</t>
+  </si>
+  <si>
+    <t>CE003C</t>
+  </si>
+  <si>
+    <t>Capricious</t>
+  </si>
+  <si>
+    <t>B90025</t>
+  </si>
+  <si>
+    <t>Wicked</t>
+  </si>
+  <si>
+    <t>Royal</t>
+  </si>
+  <si>
+    <t>Captivated</t>
+  </si>
+  <si>
+    <t>C37C77</t>
+  </si>
+  <si>
+    <t>Charmed</t>
+  </si>
+  <si>
+    <t>C86F6A</t>
+  </si>
+  <si>
+    <t>Golden</t>
+  </si>
+  <si>
+    <t>D26658</t>
+  </si>
+  <si>
+    <t>Awestruck</t>
+  </si>
+  <si>
+    <t>A06169</t>
+  </si>
+  <si>
+    <t>A84B4D</t>
+  </si>
+  <si>
+    <t>Peppy</t>
+  </si>
+  <si>
+    <t>Punchy</t>
+  </si>
+  <si>
+    <t>Keen</t>
+  </si>
+  <si>
+    <t>BA463B</t>
+  </si>
+  <si>
+    <t>963A2D</t>
+  </si>
+  <si>
+    <t>Fearless</t>
+  </si>
+  <si>
+    <t>Charged</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>4B262B</t>
+  </si>
+  <si>
+    <t>2F1D23</t>
+  </si>
+  <si>
+    <t>A00082</t>
+  </si>
+  <si>
+    <t>A00083</t>
+  </si>
+  <si>
+    <t>A00084</t>
+  </si>
+  <si>
+    <t>A00085</t>
+  </si>
+  <si>
+    <t>A00086</t>
+  </si>
+  <si>
+    <t>A00087</t>
+  </si>
+  <si>
+    <t>A00088</t>
+  </si>
+  <si>
+    <t>A00089</t>
+  </si>
+  <si>
+    <t>Color Sensation Ultimatte Matte Intense</t>
+  </si>
+  <si>
+    <t>color_sensational_ultimattes</t>
+  </si>
+  <si>
+    <t>More Scarlet</t>
+  </si>
+  <si>
+    <t>CC2229</t>
+  </si>
+  <si>
+    <t>More Taupe</t>
+  </si>
+  <si>
+    <t>A24D44</t>
+  </si>
+  <si>
+    <t>D7817C</t>
+  </si>
+  <si>
+    <t>More Auburn</t>
+  </si>
+  <si>
+    <t>More Almond</t>
+  </si>
+  <si>
+    <t>AF6054</t>
+  </si>
+  <si>
+    <t>C44757</t>
+  </si>
+  <si>
+    <t>More Blush</t>
+  </si>
+  <si>
+    <t>B64133</t>
+  </si>
+  <si>
+    <t>More Rust</t>
+  </si>
+  <si>
+    <t>A00090</t>
+  </si>
+  <si>
+    <t>A00091</t>
+  </si>
+  <si>
+    <t>A00092</t>
+  </si>
+  <si>
+    <t>A00093</t>
+  </si>
+  <si>
+    <t>A00094</t>
+  </si>
+  <si>
+    <t>A00095</t>
+  </si>
+  <si>
+    <t>Midtown Pink</t>
+  </si>
+  <si>
+    <t>A85345</t>
+  </si>
+  <si>
+    <t>Madison Red</t>
+  </si>
+  <si>
+    <t>C3583A</t>
+  </si>
+  <si>
+    <t>Brookyln Bare</t>
+  </si>
+  <si>
+    <t>93312D</t>
+  </si>
+  <si>
+    <t>East Village Rose</t>
+  </si>
+  <si>
+    <t>85160A</t>
+  </si>
+  <si>
+    <t>Noho Amber</t>
+  </si>
+  <si>
+    <t>A00096</t>
+  </si>
+  <si>
+    <t>A00097</t>
+  </si>
+  <si>
+    <t>A00098</t>
+  </si>
+  <si>
+    <t>A00099</t>
+  </si>
+  <si>
+    <t>A00100</t>
+  </si>
+  <si>
+    <t>color_sensational_bricks</t>
+  </si>
+  <si>
+    <t>Color Sensation The Bricks City Heat</t>
   </si>
 </sst>
 </file>
@@ -285,10 +1011,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -605,18 +1334,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EEC25AA-D88A-064C-89E7-319327594E20}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" style="1"/>
     <col min="2" max="3" width="59.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="115" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="40" style="1"/>
+    <col min="4" max="4" width="115" style="2" customWidth="1"/>
+    <col min="5" max="5" width="40" style="2"/>
+    <col min="6" max="16384" width="40" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -629,10 +1359,10 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -646,10 +1376,10 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -663,10 +1393,10 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -680,7 +1410,7 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="2">
@@ -697,10 +1427,10 @@
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -714,10 +1444,10 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -731,10 +1461,10 @@
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -748,10 +1478,10 @@
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -765,10 +1495,10 @@
       <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -782,10 +1512,10 @@
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -799,10 +1529,10 @@
       <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -816,10 +1546,10 @@
       <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>43</v>
       </c>
     </row>
@@ -833,10 +1563,10 @@
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -850,10 +1580,10 @@
       <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -867,10 +1597,10 @@
       <c r="C15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -884,10 +1614,10 @@
       <c r="C16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>60</v>
       </c>
     </row>
@@ -901,10 +1631,10 @@
       <c r="C17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="D17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -918,10 +1648,10 @@
       <c r="C18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>62</v>
       </c>
     </row>
@@ -935,10 +1665,10 @@
       <c r="C19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>63</v>
       </c>
     </row>
@@ -952,7 +1682,7 @@
       <c r="C20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E20" s="2">
@@ -969,11 +1699,1371 @@
       <c r="C21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="2">
+        <v>933128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" s="2">
+        <v>783327</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E44" s="2">
+        <v>682013</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E45" s="2">
+        <v>863224</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E46" s="2">
+        <v>611816</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E47" s="2">
+        <v>810604</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E69" s="2">
+        <v>894940</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E80" s="2">
+        <v>770615</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E86" s="2">
+        <v>965952</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E98" s="2">
+        <v>842916</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>